<commit_message>
the admin page reequest
</commit_message>
<xml_diff>
--- a/admin/Examinees_List.xlsx
+++ b/admin/Examinees_List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>ID</t>
   </si>
@@ -39,18 +39,6 @@
   </si>
   <si>
     <t>Institution</t>
-  </si>
-  <si>
-    <t>Yohannes Assefa</t>
-  </si>
-  <si>
-    <t>yohannes@mail.com</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>D</t>
   </si>
 </sst>
 </file>
@@ -389,7 +377,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,54 +409,6 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
-        <v>174</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2"/>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
-        <v>175</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3"/>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the response for the request send by the user to add the I, D, C
</commit_message>
<xml_diff>
--- a/admin/Examinees_List.xlsx
+++ b/admin/Examinees_List.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -39,6 +39,42 @@
   </si>
   <si>
     <t>Institution</t>
+  </si>
+  <si>
+    <t>Yohannes Fantahun</t>
+  </si>
+  <si>
+    <t>fantish@mail.com</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Unity University College</t>
+  </si>
+  <si>
+    <t>test person</t>
+  </si>
+  <si>
+    <t>test@mail.com</t>
+  </si>
+  <si>
+    <t>Addis Ababa University</t>
+  </si>
+  <si>
+    <t>Abex Abelew</t>
+  </si>
+  <si>
+    <t>abex@mail.com</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -377,7 +413,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -409,6 +445,84 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>